<commit_message>
Guia 1 Est 115
</commit_message>
<xml_diff>
--- a/Notas_Master.xlsx
+++ b/Notas_Master.xlsx
@@ -17371,7 +17371,7 @@
         </is>
       </c>
       <c r="H36" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="37">
@@ -18055,7 +18055,7 @@
         </is>
       </c>
       <c r="H54" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="55">
@@ -19765,7 +19765,7 @@
         </is>
       </c>
       <c r="H99" t="n">
-        <v>1</v>
+        <v>3.5</v>
       </c>
     </row>
     <row r="100">
@@ -20449,7 +20449,7 @@
         </is>
       </c>
       <c r="H117" t="n">
-        <v>1</v>
+        <v>3.9</v>
       </c>
     </row>
     <row r="118">
@@ -21133,7 +21133,7 @@
         </is>
       </c>
       <c r="H135" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="136">
@@ -21817,7 +21817,7 @@
         </is>
       </c>
       <c r="H153" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="154">
@@ -22843,7 +22843,7 @@
         </is>
       </c>
       <c r="H180" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="181">
@@ -23869,7 +23869,7 @@
         </is>
       </c>
       <c r="H207" t="n">
-        <v>1</v>
+        <v>3.3</v>
       </c>
     </row>
     <row r="208">
@@ -24211,7 +24211,7 @@
         </is>
       </c>
       <c r="H216" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="217">
@@ -25921,7 +25921,7 @@
         </is>
       </c>
       <c r="H261" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="262">
@@ -28657,7 +28657,7 @@
         </is>
       </c>
       <c r="H333" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="334">
@@ -30419,7 +30419,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H208"/>
+  <dimension ref="A1:H217"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1:H1"/>
@@ -31647,7 +31647,7 @@
         </is>
       </c>
       <c r="H32" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="33">
@@ -32331,7 +32331,7 @@
         </is>
       </c>
       <c r="H50" t="n">
-        <v>1</v>
+        <v>4.2</v>
       </c>
     </row>
     <row r="51">
@@ -32673,7 +32673,7 @@
         </is>
       </c>
       <c r="H59" t="n">
-        <v>1</v>
+        <v>4.5</v>
       </c>
     </row>
     <row r="60">
@@ -35067,7 +35067,7 @@
         </is>
       </c>
       <c r="H122" t="n">
-        <v>1</v>
+        <v>4.5</v>
       </c>
     </row>
     <row r="123">
@@ -35409,7 +35409,7 @@
         </is>
       </c>
       <c r="H131" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="132">
@@ -35751,7 +35751,7 @@
         </is>
       </c>
       <c r="H140" t="n">
-        <v>1</v>
+        <v>4.3</v>
       </c>
     </row>
     <row r="141">
@@ -36636,17 +36636,17 @@
       </c>
       <c r="B164" t="inlineStr">
         <is>
-          <t>210307</t>
+          <t>240667</t>
         </is>
       </c>
       <c r="C164" t="inlineStr">
         <is>
-          <t>4586271</t>
+          <t>1035974995</t>
         </is>
       </c>
       <c r="D164" t="inlineStr">
         <is>
-          <t>PLANCHEZ URDANETA, GLEINNYS DE LA CHIQUINQUIRA</t>
+          <t>OSPINA ESCOBAR, SEBASTIAN</t>
         </is>
       </c>
       <c r="E164" t="n">
@@ -36674,17 +36674,17 @@
       </c>
       <c r="B165" t="inlineStr">
         <is>
-          <t>210307</t>
+          <t>240667</t>
         </is>
       </c>
       <c r="C165" t="inlineStr">
         <is>
-          <t>4586271</t>
+          <t>1035974995</t>
         </is>
       </c>
       <c r="D165" t="inlineStr">
         <is>
-          <t>PLANCHEZ URDANETA, GLEINNYS DE LA CHIQUINQUIRA</t>
+          <t>OSPINA ESCOBAR, SEBASTIAN</t>
         </is>
       </c>
       <c r="E165" t="n">
@@ -36701,7 +36701,7 @@
         </is>
       </c>
       <c r="H165" t="n">
-        <v>3.5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="166">
@@ -36712,17 +36712,17 @@
       </c>
       <c r="B166" t="inlineStr">
         <is>
-          <t>210307</t>
+          <t>240667</t>
         </is>
       </c>
       <c r="C166" t="inlineStr">
         <is>
-          <t>4586271</t>
+          <t>1035974995</t>
         </is>
       </c>
       <c r="D166" t="inlineStr">
         <is>
-          <t>PLANCHEZ URDANETA, GLEINNYS DE LA CHIQUINQUIRA</t>
+          <t>OSPINA ESCOBAR, SEBASTIAN</t>
         </is>
       </c>
       <c r="E166" t="n">
@@ -36739,7 +36739,7 @@
         </is>
       </c>
       <c r="H166" t="n">
-        <v>1</v>
+        <v>3.3</v>
       </c>
     </row>
     <row r="167">
@@ -36750,17 +36750,17 @@
       </c>
       <c r="B167" t="inlineStr">
         <is>
-          <t>210307</t>
+          <t>240667</t>
         </is>
       </c>
       <c r="C167" t="inlineStr">
         <is>
-          <t>4586271</t>
+          <t>1035974995</t>
         </is>
       </c>
       <c r="D167" t="inlineStr">
         <is>
-          <t>PLANCHEZ URDANETA, GLEINNYS DE LA CHIQUINQUIRA</t>
+          <t>OSPINA ESCOBAR, SEBASTIAN</t>
         </is>
       </c>
       <c r="E167" t="n">
@@ -36788,17 +36788,17 @@
       </c>
       <c r="B168" t="inlineStr">
         <is>
-          <t>210307</t>
+          <t>240667</t>
         </is>
       </c>
       <c r="C168" t="inlineStr">
         <is>
-          <t>4586271</t>
+          <t>1035974995</t>
         </is>
       </c>
       <c r="D168" t="inlineStr">
         <is>
-          <t>PLANCHEZ URDANETA, GLEINNYS DE LA CHIQUINQUIRA</t>
+          <t>OSPINA ESCOBAR, SEBASTIAN</t>
         </is>
       </c>
       <c r="E168" t="n">
@@ -36815,7 +36815,7 @@
         </is>
       </c>
       <c r="H168" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="169">
@@ -36826,17 +36826,17 @@
       </c>
       <c r="B169" t="inlineStr">
         <is>
-          <t>210307</t>
+          <t>240667</t>
         </is>
       </c>
       <c r="C169" t="inlineStr">
         <is>
-          <t>4586271</t>
+          <t>1035974995</t>
         </is>
       </c>
       <c r="D169" t="inlineStr">
         <is>
-          <t>PLANCHEZ URDANETA, GLEINNYS DE LA CHIQUINQUIRA</t>
+          <t>OSPINA ESCOBAR, SEBASTIAN</t>
         </is>
       </c>
       <c r="E169" t="n">
@@ -36853,7 +36853,7 @@
         </is>
       </c>
       <c r="H169" t="n">
-        <v>3</v>
+        <v>3.8</v>
       </c>
     </row>
     <row r="170">
@@ -36864,17 +36864,17 @@
       </c>
       <c r="B170" t="inlineStr">
         <is>
-          <t>210307</t>
+          <t>240667</t>
         </is>
       </c>
       <c r="C170" t="inlineStr">
         <is>
-          <t>4586271</t>
+          <t>1035974995</t>
         </is>
       </c>
       <c r="D170" t="inlineStr">
         <is>
-          <t>PLANCHEZ URDANETA, GLEINNYS DE LA CHIQUINQUIRA</t>
+          <t>OSPINA ESCOBAR, SEBASTIAN</t>
         </is>
       </c>
       <c r="E170" t="n">
@@ -36902,17 +36902,17 @@
       </c>
       <c r="B171" t="inlineStr">
         <is>
-          <t>210307</t>
+          <t>240667</t>
         </is>
       </c>
       <c r="C171" t="inlineStr">
         <is>
-          <t>4586271</t>
+          <t>1035974995</t>
         </is>
       </c>
       <c r="D171" t="inlineStr">
         <is>
-          <t>PLANCHEZ URDANETA, GLEINNYS DE LA CHIQUINQUIRA</t>
+          <t>OSPINA ESCOBAR, SEBASTIAN</t>
         </is>
       </c>
       <c r="E171" t="n">
@@ -36940,17 +36940,17 @@
       </c>
       <c r="B172" t="inlineStr">
         <is>
-          <t>210307</t>
+          <t>240667</t>
         </is>
       </c>
       <c r="C172" t="inlineStr">
         <is>
-          <t>4586271</t>
+          <t>1035974995</t>
         </is>
       </c>
       <c r="D172" t="inlineStr">
         <is>
-          <t>PLANCHEZ URDANETA, GLEINNYS DE LA CHIQUINQUIRA</t>
+          <t>OSPINA ESCOBAR, SEBASTIAN</t>
         </is>
       </c>
       <c r="E172" t="n">
@@ -36967,7 +36967,7 @@
         </is>
       </c>
       <c r="H172" t="n">
-        <v>2.6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="173">
@@ -36978,17 +36978,17 @@
       </c>
       <c r="B173" t="inlineStr">
         <is>
-          <t>210167</t>
+          <t>210307</t>
         </is>
       </c>
       <c r="C173" t="inlineStr">
         <is>
-          <t>1078637012</t>
+          <t>4586271</t>
         </is>
       </c>
       <c r="D173" t="inlineStr">
         <is>
-          <t>ROLDAN  GALLO, HALAN STIVEN</t>
+          <t>PLANCHEZ URDANETA, GLEINNYS DE LA CHIQUINQUIRA</t>
         </is>
       </c>
       <c r="E173" t="n">
@@ -37005,7 +37005,7 @@
         </is>
       </c>
       <c r="H173" t="n">
-        <v>3.5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="174">
@@ -37016,17 +37016,17 @@
       </c>
       <c r="B174" t="inlineStr">
         <is>
-          <t>210167</t>
+          <t>210307</t>
         </is>
       </c>
       <c r="C174" t="inlineStr">
         <is>
-          <t>1078637012</t>
+          <t>4586271</t>
         </is>
       </c>
       <c r="D174" t="inlineStr">
         <is>
-          <t>ROLDAN  GALLO, HALAN STIVEN</t>
+          <t>PLANCHEZ URDANETA, GLEINNYS DE LA CHIQUINQUIRA</t>
         </is>
       </c>
       <c r="E174" t="n">
@@ -37043,7 +37043,7 @@
         </is>
       </c>
       <c r="H174" t="n">
-        <v>3</v>
+        <v>3.5</v>
       </c>
     </row>
     <row r="175">
@@ -37054,17 +37054,17 @@
       </c>
       <c r="B175" t="inlineStr">
         <is>
-          <t>210167</t>
+          <t>210307</t>
         </is>
       </c>
       <c r="C175" t="inlineStr">
         <is>
-          <t>1078637012</t>
+          <t>4586271</t>
         </is>
       </c>
       <c r="D175" t="inlineStr">
         <is>
-          <t>ROLDAN  GALLO, HALAN STIVEN</t>
+          <t>PLANCHEZ URDANETA, GLEINNYS DE LA CHIQUINQUIRA</t>
         </is>
       </c>
       <c r="E175" t="n">
@@ -37092,17 +37092,17 @@
       </c>
       <c r="B176" t="inlineStr">
         <is>
-          <t>210167</t>
+          <t>210307</t>
         </is>
       </c>
       <c r="C176" t="inlineStr">
         <is>
-          <t>1078637012</t>
+          <t>4586271</t>
         </is>
       </c>
       <c r="D176" t="inlineStr">
         <is>
-          <t>ROLDAN  GALLO, HALAN STIVEN</t>
+          <t>PLANCHEZ URDANETA, GLEINNYS DE LA CHIQUINQUIRA</t>
         </is>
       </c>
       <c r="E176" t="n">
@@ -37119,7 +37119,7 @@
         </is>
       </c>
       <c r="H176" t="n">
-        <v>1</v>
+        <v>4.2</v>
       </c>
     </row>
     <row r="177">
@@ -37130,17 +37130,17 @@
       </c>
       <c r="B177" t="inlineStr">
         <is>
-          <t>210167</t>
+          <t>210307</t>
         </is>
       </c>
       <c r="C177" t="inlineStr">
         <is>
-          <t>1078637012</t>
+          <t>4586271</t>
         </is>
       </c>
       <c r="D177" t="inlineStr">
         <is>
-          <t>ROLDAN  GALLO, HALAN STIVEN</t>
+          <t>PLANCHEZ URDANETA, GLEINNYS DE LA CHIQUINQUIRA</t>
         </is>
       </c>
       <c r="E177" t="n">
@@ -37157,7 +37157,7 @@
         </is>
       </c>
       <c r="H177" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="178">
@@ -37168,17 +37168,17 @@
       </c>
       <c r="B178" t="inlineStr">
         <is>
-          <t>210167</t>
+          <t>210307</t>
         </is>
       </c>
       <c r="C178" t="inlineStr">
         <is>
-          <t>1078637012</t>
+          <t>4586271</t>
         </is>
       </c>
       <c r="D178" t="inlineStr">
         <is>
-          <t>ROLDAN  GALLO, HALAN STIVEN</t>
+          <t>PLANCHEZ URDANETA, GLEINNYS DE LA CHIQUINQUIRA</t>
         </is>
       </c>
       <c r="E178" t="n">
@@ -37195,7 +37195,7 @@
         </is>
       </c>
       <c r="H178" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="179">
@@ -37206,17 +37206,17 @@
       </c>
       <c r="B179" t="inlineStr">
         <is>
-          <t>210167</t>
+          <t>210307</t>
         </is>
       </c>
       <c r="C179" t="inlineStr">
         <is>
-          <t>1078637012</t>
+          <t>4586271</t>
         </is>
       </c>
       <c r="D179" t="inlineStr">
         <is>
-          <t>ROLDAN  GALLO, HALAN STIVEN</t>
+          <t>PLANCHEZ URDANETA, GLEINNYS DE LA CHIQUINQUIRA</t>
         </is>
       </c>
       <c r="E179" t="n">
@@ -37244,17 +37244,17 @@
       </c>
       <c r="B180" t="inlineStr">
         <is>
-          <t>210167</t>
+          <t>210307</t>
         </is>
       </c>
       <c r="C180" t="inlineStr">
         <is>
-          <t>1078637012</t>
+          <t>4586271</t>
         </is>
       </c>
       <c r="D180" t="inlineStr">
         <is>
-          <t>ROLDAN  GALLO, HALAN STIVEN</t>
+          <t>PLANCHEZ URDANETA, GLEINNYS DE LA CHIQUINQUIRA</t>
         </is>
       </c>
       <c r="E180" t="n">
@@ -37282,17 +37282,17 @@
       </c>
       <c r="B181" t="inlineStr">
         <is>
-          <t>210167</t>
+          <t>210307</t>
         </is>
       </c>
       <c r="C181" t="inlineStr">
         <is>
-          <t>1078637012</t>
+          <t>4586271</t>
         </is>
       </c>
       <c r="D181" t="inlineStr">
         <is>
-          <t>ROLDAN  GALLO, HALAN STIVEN</t>
+          <t>PLANCHEZ URDANETA, GLEINNYS DE LA CHIQUINQUIRA</t>
         </is>
       </c>
       <c r="E181" t="n">
@@ -37309,7 +37309,7 @@
         </is>
       </c>
       <c r="H181" t="n">
-        <v>3</v>
+        <v>2.6</v>
       </c>
     </row>
     <row r="182">
@@ -37320,17 +37320,17 @@
       </c>
       <c r="B182" t="inlineStr">
         <is>
-          <t>210019</t>
+          <t>210167</t>
         </is>
       </c>
       <c r="C182" t="inlineStr">
         <is>
-          <t>1038263883</t>
+          <t>1078637012</t>
         </is>
       </c>
       <c r="D182" t="inlineStr">
         <is>
-          <t>TABORDA GAVIRIA, JERONIMO</t>
+          <t>ROLDAN  GALLO, HALAN STIVEN</t>
         </is>
       </c>
       <c r="E182" t="n">
@@ -37347,7 +37347,7 @@
         </is>
       </c>
       <c r="H182" t="n">
-        <v>5</v>
+        <v>3.5</v>
       </c>
     </row>
     <row r="183">
@@ -37358,17 +37358,17 @@
       </c>
       <c r="B183" t="inlineStr">
         <is>
-          <t>210019</t>
+          <t>210167</t>
         </is>
       </c>
       <c r="C183" t="inlineStr">
         <is>
-          <t>1038263883</t>
+          <t>1078637012</t>
         </is>
       </c>
       <c r="D183" t="inlineStr">
         <is>
-          <t>TABORDA GAVIRIA, JERONIMO</t>
+          <t>ROLDAN  GALLO, HALAN STIVEN</t>
         </is>
       </c>
       <c r="E183" t="n">
@@ -37385,7 +37385,7 @@
         </is>
       </c>
       <c r="H183" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="184">
@@ -37396,17 +37396,17 @@
       </c>
       <c r="B184" t="inlineStr">
         <is>
-          <t>210019</t>
+          <t>210167</t>
         </is>
       </c>
       <c r="C184" t="inlineStr">
         <is>
-          <t>1038263883</t>
+          <t>1078637012</t>
         </is>
       </c>
       <c r="D184" t="inlineStr">
         <is>
-          <t>TABORDA GAVIRIA, JERONIMO</t>
+          <t>ROLDAN  GALLO, HALAN STIVEN</t>
         </is>
       </c>
       <c r="E184" t="n">
@@ -37423,7 +37423,7 @@
         </is>
       </c>
       <c r="H184" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="185">
@@ -37434,17 +37434,17 @@
       </c>
       <c r="B185" t="inlineStr">
         <is>
-          <t>210019</t>
+          <t>210167</t>
         </is>
       </c>
       <c r="C185" t="inlineStr">
         <is>
-          <t>1038263883</t>
+          <t>1078637012</t>
         </is>
       </c>
       <c r="D185" t="inlineStr">
         <is>
-          <t>TABORDA GAVIRIA, JERONIMO</t>
+          <t>ROLDAN  GALLO, HALAN STIVEN</t>
         </is>
       </c>
       <c r="E185" t="n">
@@ -37472,17 +37472,17 @@
       </c>
       <c r="B186" t="inlineStr">
         <is>
-          <t>210019</t>
+          <t>210167</t>
         </is>
       </c>
       <c r="C186" t="inlineStr">
         <is>
-          <t>1038263883</t>
+          <t>1078637012</t>
         </is>
       </c>
       <c r="D186" t="inlineStr">
         <is>
-          <t>TABORDA GAVIRIA, JERONIMO</t>
+          <t>ROLDAN  GALLO, HALAN STIVEN</t>
         </is>
       </c>
       <c r="E186" t="n">
@@ -37499,7 +37499,7 @@
         </is>
       </c>
       <c r="H186" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="187">
@@ -37510,17 +37510,17 @@
       </c>
       <c r="B187" t="inlineStr">
         <is>
-          <t>210019</t>
+          <t>210167</t>
         </is>
       </c>
       <c r="C187" t="inlineStr">
         <is>
-          <t>1038263883</t>
+          <t>1078637012</t>
         </is>
       </c>
       <c r="D187" t="inlineStr">
         <is>
-          <t>TABORDA GAVIRIA, JERONIMO</t>
+          <t>ROLDAN  GALLO, HALAN STIVEN</t>
         </is>
       </c>
       <c r="E187" t="n">
@@ -37537,7 +37537,7 @@
         </is>
       </c>
       <c r="H187" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="188">
@@ -37548,17 +37548,17 @@
       </c>
       <c r="B188" t="inlineStr">
         <is>
-          <t>210019</t>
+          <t>210167</t>
         </is>
       </c>
       <c r="C188" t="inlineStr">
         <is>
-          <t>1038263883</t>
+          <t>1078637012</t>
         </is>
       </c>
       <c r="D188" t="inlineStr">
         <is>
-          <t>TABORDA GAVIRIA, JERONIMO</t>
+          <t>ROLDAN  GALLO, HALAN STIVEN</t>
         </is>
       </c>
       <c r="E188" t="n">
@@ -37586,17 +37586,17 @@
       </c>
       <c r="B189" t="inlineStr">
         <is>
-          <t>210019</t>
+          <t>210167</t>
         </is>
       </c>
       <c r="C189" t="inlineStr">
         <is>
-          <t>1038263883</t>
+          <t>1078637012</t>
         </is>
       </c>
       <c r="D189" t="inlineStr">
         <is>
-          <t>TABORDA GAVIRIA, JERONIMO</t>
+          <t>ROLDAN  GALLO, HALAN STIVEN</t>
         </is>
       </c>
       <c r="E189" t="n">
@@ -37624,17 +37624,17 @@
       </c>
       <c r="B190" t="inlineStr">
         <is>
-          <t>210019</t>
+          <t>210167</t>
         </is>
       </c>
       <c r="C190" t="inlineStr">
         <is>
-          <t>1038263883</t>
+          <t>1078637012</t>
         </is>
       </c>
       <c r="D190" t="inlineStr">
         <is>
-          <t>TABORDA GAVIRIA, JERONIMO</t>
+          <t>ROLDAN  GALLO, HALAN STIVEN</t>
         </is>
       </c>
       <c r="E190" t="n">
@@ -37651,7 +37651,7 @@
         </is>
       </c>
       <c r="H190" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="191">
@@ -37662,17 +37662,17 @@
       </c>
       <c r="B191" t="inlineStr">
         <is>
-          <t>150447</t>
+          <t>210019</t>
         </is>
       </c>
       <c r="C191" t="inlineStr">
         <is>
-          <t>N37624903911</t>
+          <t>1038263883</t>
         </is>
       </c>
       <c r="D191" t="inlineStr">
         <is>
-          <t>YU LUO, WENJIN</t>
+          <t>TABORDA GAVIRIA, JERONIMO</t>
         </is>
       </c>
       <c r="E191" t="n">
@@ -37700,17 +37700,17 @@
       </c>
       <c r="B192" t="inlineStr">
         <is>
-          <t>150447</t>
+          <t>210019</t>
         </is>
       </c>
       <c r="C192" t="inlineStr">
         <is>
-          <t>N37624903911</t>
+          <t>1038263883</t>
         </is>
       </c>
       <c r="D192" t="inlineStr">
         <is>
-          <t>YU LUO, WENJIN</t>
+          <t>TABORDA GAVIRIA, JERONIMO</t>
         </is>
       </c>
       <c r="E192" t="n">
@@ -37727,7 +37727,7 @@
         </is>
       </c>
       <c r="H192" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="193">
@@ -37738,17 +37738,17 @@
       </c>
       <c r="B193" t="inlineStr">
         <is>
-          <t>150447</t>
+          <t>210019</t>
         </is>
       </c>
       <c r="C193" t="inlineStr">
         <is>
-          <t>N37624903911</t>
+          <t>1038263883</t>
         </is>
       </c>
       <c r="D193" t="inlineStr">
         <is>
-          <t>YU LUO, WENJIN</t>
+          <t>TABORDA GAVIRIA, JERONIMO</t>
         </is>
       </c>
       <c r="E193" t="n">
@@ -37765,7 +37765,7 @@
         </is>
       </c>
       <c r="H193" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="194">
@@ -37776,17 +37776,17 @@
       </c>
       <c r="B194" t="inlineStr">
         <is>
-          <t>150447</t>
+          <t>210019</t>
         </is>
       </c>
       <c r="C194" t="inlineStr">
         <is>
-          <t>N37624903911</t>
+          <t>1038263883</t>
         </is>
       </c>
       <c r="D194" t="inlineStr">
         <is>
-          <t>YU LUO, WENJIN</t>
+          <t>TABORDA GAVIRIA, JERONIMO</t>
         </is>
       </c>
       <c r="E194" t="n">
@@ -37814,17 +37814,17 @@
       </c>
       <c r="B195" t="inlineStr">
         <is>
-          <t>150447</t>
+          <t>210019</t>
         </is>
       </c>
       <c r="C195" t="inlineStr">
         <is>
-          <t>N37624903911</t>
+          <t>1038263883</t>
         </is>
       </c>
       <c r="D195" t="inlineStr">
         <is>
-          <t>YU LUO, WENJIN</t>
+          <t>TABORDA GAVIRIA, JERONIMO</t>
         </is>
       </c>
       <c r="E195" t="n">
@@ -37841,7 +37841,7 @@
         </is>
       </c>
       <c r="H195" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="196">
@@ -37852,17 +37852,17 @@
       </c>
       <c r="B196" t="inlineStr">
         <is>
-          <t>150447</t>
+          <t>210019</t>
         </is>
       </c>
       <c r="C196" t="inlineStr">
         <is>
-          <t>N37624903911</t>
+          <t>1038263883</t>
         </is>
       </c>
       <c r="D196" t="inlineStr">
         <is>
-          <t>YU LUO, WENJIN</t>
+          <t>TABORDA GAVIRIA, JERONIMO</t>
         </is>
       </c>
       <c r="E196" t="n">
@@ -37879,7 +37879,7 @@
         </is>
       </c>
       <c r="H196" t="n">
-        <v>4.7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="197">
@@ -37890,17 +37890,17 @@
       </c>
       <c r="B197" t="inlineStr">
         <is>
-          <t>150447</t>
+          <t>210019</t>
         </is>
       </c>
       <c r="C197" t="inlineStr">
         <is>
-          <t>N37624903911</t>
+          <t>1038263883</t>
         </is>
       </c>
       <c r="D197" t="inlineStr">
         <is>
-          <t>YU LUO, WENJIN</t>
+          <t>TABORDA GAVIRIA, JERONIMO</t>
         </is>
       </c>
       <c r="E197" t="n">
@@ -37928,17 +37928,17 @@
       </c>
       <c r="B198" t="inlineStr">
         <is>
-          <t>150447</t>
+          <t>210019</t>
         </is>
       </c>
       <c r="C198" t="inlineStr">
         <is>
-          <t>N37624903911</t>
+          <t>1038263883</t>
         </is>
       </c>
       <c r="D198" t="inlineStr">
         <is>
-          <t>YU LUO, WENJIN</t>
+          <t>TABORDA GAVIRIA, JERONIMO</t>
         </is>
       </c>
       <c r="E198" t="n">
@@ -37966,17 +37966,17 @@
       </c>
       <c r="B199" t="inlineStr">
         <is>
-          <t>150447</t>
+          <t>210019</t>
         </is>
       </c>
       <c r="C199" t="inlineStr">
         <is>
-          <t>N37624903911</t>
+          <t>1038263883</t>
         </is>
       </c>
       <c r="D199" t="inlineStr">
         <is>
-          <t>YU LUO, WENJIN</t>
+          <t>TABORDA GAVIRIA, JERONIMO</t>
         </is>
       </c>
       <c r="E199" t="n">
@@ -37993,7 +37993,7 @@
         </is>
       </c>
       <c r="H199" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="200">
@@ -38004,17 +38004,17 @@
       </c>
       <c r="B200" t="inlineStr">
         <is>
-          <t>220244</t>
+          <t>150447</t>
         </is>
       </c>
       <c r="C200" t="inlineStr">
         <is>
-          <t>1038263973</t>
+          <t>N37624903911</t>
         </is>
       </c>
       <c r="D200" t="inlineStr">
         <is>
-          <t>ZAPATA  GONZALEZ, NYCHOLL</t>
+          <t>YU LUO, WENJIN</t>
         </is>
       </c>
       <c r="E200" t="n">
@@ -38031,7 +38031,7 @@
         </is>
       </c>
       <c r="H200" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="201">
@@ -38042,17 +38042,17 @@
       </c>
       <c r="B201" t="inlineStr">
         <is>
-          <t>220244</t>
+          <t>150447</t>
         </is>
       </c>
       <c r="C201" t="inlineStr">
         <is>
-          <t>1038263973</t>
+          <t>N37624903911</t>
         </is>
       </c>
       <c r="D201" t="inlineStr">
         <is>
-          <t>ZAPATA  GONZALEZ, NYCHOLL</t>
+          <t>YU LUO, WENJIN</t>
         </is>
       </c>
       <c r="E201" t="n">
@@ -38080,17 +38080,17 @@
       </c>
       <c r="B202" t="inlineStr">
         <is>
-          <t>220244</t>
+          <t>150447</t>
         </is>
       </c>
       <c r="C202" t="inlineStr">
         <is>
-          <t>1038263973</t>
+          <t>N37624903911</t>
         </is>
       </c>
       <c r="D202" t="inlineStr">
         <is>
-          <t>ZAPATA  GONZALEZ, NYCHOLL</t>
+          <t>YU LUO, WENJIN</t>
         </is>
       </c>
       <c r="E202" t="n">
@@ -38107,7 +38107,7 @@
         </is>
       </c>
       <c r="H202" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="203">
@@ -38118,17 +38118,17 @@
       </c>
       <c r="B203" t="inlineStr">
         <is>
-          <t>220244</t>
+          <t>150447</t>
         </is>
       </c>
       <c r="C203" t="inlineStr">
         <is>
-          <t>1038263973</t>
+          <t>N37624903911</t>
         </is>
       </c>
       <c r="D203" t="inlineStr">
         <is>
-          <t>ZAPATA  GONZALEZ, NYCHOLL</t>
+          <t>YU LUO, WENJIN</t>
         </is>
       </c>
       <c r="E203" t="n">
@@ -38145,7 +38145,7 @@
         </is>
       </c>
       <c r="H203" t="n">
-        <v>1</v>
+        <v>4.3</v>
       </c>
     </row>
     <row r="204">
@@ -38156,17 +38156,17 @@
       </c>
       <c r="B204" t="inlineStr">
         <is>
-          <t>220244</t>
+          <t>150447</t>
         </is>
       </c>
       <c r="C204" t="inlineStr">
         <is>
-          <t>1038263973</t>
+          <t>N37624903911</t>
         </is>
       </c>
       <c r="D204" t="inlineStr">
         <is>
-          <t>ZAPATA  GONZALEZ, NYCHOLL</t>
+          <t>YU LUO, WENJIN</t>
         </is>
       </c>
       <c r="E204" t="n">
@@ -38183,7 +38183,7 @@
         </is>
       </c>
       <c r="H204" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="205">
@@ -38194,17 +38194,17 @@
       </c>
       <c r="B205" t="inlineStr">
         <is>
-          <t>220244</t>
+          <t>150447</t>
         </is>
       </c>
       <c r="C205" t="inlineStr">
         <is>
-          <t>1038263973</t>
+          <t>N37624903911</t>
         </is>
       </c>
       <c r="D205" t="inlineStr">
         <is>
-          <t>ZAPATA  GONZALEZ, NYCHOLL</t>
+          <t>YU LUO, WENJIN</t>
         </is>
       </c>
       <c r="E205" t="n">
@@ -38221,7 +38221,7 @@
         </is>
       </c>
       <c r="H205" t="n">
-        <v>1</v>
+        <v>4.7</v>
       </c>
     </row>
     <row r="206">
@@ -38232,17 +38232,17 @@
       </c>
       <c r="B206" t="inlineStr">
         <is>
-          <t>220244</t>
+          <t>150447</t>
         </is>
       </c>
       <c r="C206" t="inlineStr">
         <is>
-          <t>1038263973</t>
+          <t>N37624903911</t>
         </is>
       </c>
       <c r="D206" t="inlineStr">
         <is>
-          <t>ZAPATA  GONZALEZ, NYCHOLL</t>
+          <t>YU LUO, WENJIN</t>
         </is>
       </c>
       <c r="E206" t="n">
@@ -38270,17 +38270,17 @@
       </c>
       <c r="B207" t="inlineStr">
         <is>
-          <t>220244</t>
+          <t>150447</t>
         </is>
       </c>
       <c r="C207" t="inlineStr">
         <is>
-          <t>1038263973</t>
+          <t>N37624903911</t>
         </is>
       </c>
       <c r="D207" t="inlineStr">
         <is>
-          <t>ZAPATA  GONZALEZ, NYCHOLL</t>
+          <t>YU LUO, WENJIN</t>
         </is>
       </c>
       <c r="E207" t="n">
@@ -38308,17 +38308,17 @@
       </c>
       <c r="B208" t="inlineStr">
         <is>
-          <t>220244</t>
+          <t>150447</t>
         </is>
       </c>
       <c r="C208" t="inlineStr">
         <is>
-          <t>1038263973</t>
+          <t>N37624903911</t>
         </is>
       </c>
       <c r="D208" t="inlineStr">
         <is>
-          <t>ZAPATA  GONZALEZ, NYCHOLL</t>
+          <t>YU LUO, WENJIN</t>
         </is>
       </c>
       <c r="E208" t="n">
@@ -38335,6 +38335,348 @@
         </is>
       </c>
       <c r="H208" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="209">
+      <c r="A209" t="inlineStr">
+        <is>
+          <t>HACER</t>
+        </is>
+      </c>
+      <c r="B209" t="inlineStr">
+        <is>
+          <t>220244</t>
+        </is>
+      </c>
+      <c r="C209" t="inlineStr">
+        <is>
+          <t>1038263973</t>
+        </is>
+      </c>
+      <c r="D209" t="inlineStr">
+        <is>
+          <t>ZAPATA  GONZALEZ, NYCHOLL</t>
+        </is>
+      </c>
+      <c r="E209" t="n">
+        <v>1</v>
+      </c>
+      <c r="F209" t="inlineStr">
+        <is>
+          <t>1.1</t>
+        </is>
+      </c>
+      <c r="G209" t="inlineStr">
+        <is>
+          <t>Taller de ángulos y Pitágoras</t>
+        </is>
+      </c>
+      <c r="H209" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="210">
+      <c r="A210" t="inlineStr">
+        <is>
+          <t>HACER</t>
+        </is>
+      </c>
+      <c r="B210" t="inlineStr">
+        <is>
+          <t>220244</t>
+        </is>
+      </c>
+      <c r="C210" t="inlineStr">
+        <is>
+          <t>1038263973</t>
+        </is>
+      </c>
+      <c r="D210" t="inlineStr">
+        <is>
+          <t>ZAPATA  GONZALEZ, NYCHOLL</t>
+        </is>
+      </c>
+      <c r="E210" t="n">
+        <v>2</v>
+      </c>
+      <c r="F210" t="inlineStr">
+        <is>
+          <t>1.3</t>
+        </is>
+      </c>
+      <c r="G210" t="inlineStr">
+        <is>
+          <t>Ejercicios de resolución de triángulos</t>
+        </is>
+      </c>
+      <c r="H210" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="211">
+      <c r="A211" t="inlineStr">
+        <is>
+          <t>HACER</t>
+        </is>
+      </c>
+      <c r="B211" t="inlineStr">
+        <is>
+          <t>220244</t>
+        </is>
+      </c>
+      <c r="C211" t="inlineStr">
+        <is>
+          <t>1038263973</t>
+        </is>
+      </c>
+      <c r="D211" t="inlineStr">
+        <is>
+          <t>ZAPATA  GONZALEZ, NYCHOLL</t>
+        </is>
+      </c>
+      <c r="E211" t="n">
+        <v>3</v>
+      </c>
+      <c r="F211" t="inlineStr">
+        <is>
+          <t>1.5</t>
+        </is>
+      </c>
+      <c r="G211" t="inlineStr">
+        <is>
+          <t>Problemas estadística (8,10)</t>
+        </is>
+      </c>
+      <c r="H211" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="212">
+      <c r="A212" t="inlineStr">
+        <is>
+          <t>HACER</t>
+        </is>
+      </c>
+      <c r="B212" t="inlineStr">
+        <is>
+          <t>220244</t>
+        </is>
+      </c>
+      <c r="C212" t="inlineStr">
+        <is>
+          <t>1038263973</t>
+        </is>
+      </c>
+      <c r="D212" t="inlineStr">
+        <is>
+          <t>ZAPATA  GONZALEZ, NYCHOLL</t>
+        </is>
+      </c>
+      <c r="E212" t="n">
+        <v>4</v>
+      </c>
+      <c r="F212" t="inlineStr">
+        <is>
+          <t>1.7</t>
+        </is>
+      </c>
+      <c r="G212" t="inlineStr">
+        <is>
+          <t>Guía 1 de estadistica</t>
+        </is>
+      </c>
+      <c r="H212" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="213">
+      <c r="A213" t="inlineStr">
+        <is>
+          <t>SABER</t>
+        </is>
+      </c>
+      <c r="B213" t="inlineStr">
+        <is>
+          <t>220244</t>
+        </is>
+      </c>
+      <c r="C213" t="inlineStr">
+        <is>
+          <t>1038263973</t>
+        </is>
+      </c>
+      <c r="D213" t="inlineStr">
+        <is>
+          <t>ZAPATA  GONZALEZ, NYCHOLL</t>
+        </is>
+      </c>
+      <c r="E213" t="n">
+        <v>7</v>
+      </c>
+      <c r="F213" t="inlineStr">
+        <is>
+          <t>2.1</t>
+        </is>
+      </c>
+      <c r="G213" t="inlineStr">
+        <is>
+          <t>Prueba tipo icfes</t>
+        </is>
+      </c>
+      <c r="H213" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="214">
+      <c r="A214" t="inlineStr">
+        <is>
+          <t>SABER</t>
+        </is>
+      </c>
+      <c r="B214" t="inlineStr">
+        <is>
+          <t>220244</t>
+        </is>
+      </c>
+      <c r="C214" t="inlineStr">
+        <is>
+          <t>1038263973</t>
+        </is>
+      </c>
+      <c r="D214" t="inlineStr">
+        <is>
+          <t>ZAPATA  GONZALEZ, NYCHOLL</t>
+        </is>
+      </c>
+      <c r="E214" t="n">
+        <v>8</v>
+      </c>
+      <c r="F214" t="inlineStr">
+        <is>
+          <t>2.3</t>
+        </is>
+      </c>
+      <c r="G214" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Problema reglas de tres</t>
+        </is>
+      </c>
+      <c r="H214" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="215">
+      <c r="A215" t="inlineStr">
+        <is>
+          <t>AUTOEVALUACIÓN</t>
+        </is>
+      </c>
+      <c r="B215" t="inlineStr">
+        <is>
+          <t>220244</t>
+        </is>
+      </c>
+      <c r="C215" t="inlineStr">
+        <is>
+          <t>1038263973</t>
+        </is>
+      </c>
+      <c r="D215" t="inlineStr">
+        <is>
+          <t>ZAPATA  GONZALEZ, NYCHOLL</t>
+        </is>
+      </c>
+      <c r="E215" t="n">
+        <v>9</v>
+      </c>
+      <c r="F215" t="inlineStr">
+        <is>
+          <t xml:space="preserve">3.1 </t>
+        </is>
+      </c>
+      <c r="G215" t="inlineStr">
+        <is>
+          <t>Autoevaluación</t>
+        </is>
+      </c>
+      <c r="H215" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="216">
+      <c r="A216" t="inlineStr">
+        <is>
+          <t>AUTOEVALUACIÓN</t>
+        </is>
+      </c>
+      <c r="B216" t="inlineStr">
+        <is>
+          <t>220244</t>
+        </is>
+      </c>
+      <c r="C216" t="inlineStr">
+        <is>
+          <t>1038263973</t>
+        </is>
+      </c>
+      <c r="D216" t="inlineStr">
+        <is>
+          <t>ZAPATA  GONZALEZ, NYCHOLL</t>
+        </is>
+      </c>
+      <c r="E216" t="n">
+        <v>10</v>
+      </c>
+      <c r="F216" t="inlineStr">
+        <is>
+          <t xml:space="preserve">3.2 </t>
+        </is>
+      </c>
+      <c r="G216" t="inlineStr">
+        <is>
+          <t>Heteroevaluación</t>
+        </is>
+      </c>
+      <c r="H216" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="217">
+      <c r="A217" t="inlineStr">
+        <is>
+          <t>PRUEBA_PERIODO</t>
+        </is>
+      </c>
+      <c r="B217" t="inlineStr">
+        <is>
+          <t>220244</t>
+        </is>
+      </c>
+      <c r="C217" t="inlineStr">
+        <is>
+          <t>1038263973</t>
+        </is>
+      </c>
+      <c r="D217" t="inlineStr">
+        <is>
+          <t>ZAPATA  GONZALEZ, NYCHOLL</t>
+        </is>
+      </c>
+      <c r="E217" t="n">
+        <v>11</v>
+      </c>
+      <c r="F217" t="inlineStr">
+        <is>
+          <t>4.1</t>
+        </is>
+      </c>
+      <c r="G217" t="inlineStr">
+        <is>
+          <t>Prueba de periodo</t>
+        </is>
+      </c>
+      <c r="H217" t="n">
         <v>2.2</v>
       </c>
     </row>

</xml_diff>